<commit_message>
Update stock data and add new stock files
🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/dumps/Stocks/BHARTI AIRTEL.xlsx
+++ b/dumps/Stocks/BHARTI AIRTEL.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB18"/>
+  <dimension ref="A1:AB19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -574,7 +574,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46059</v>
+        <v>46062</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -587,18 +587,24 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" t="n">
-        <v>2016.28</v>
+        <v>2053</v>
       </c>
       <c r="F5" t="n">
-        <v>6048.84</v>
+        <v>4135.11</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>~</t>
-        </is>
+          <t>CN#252611665409</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>4.11</v>
+      </c>
+      <c r="I5" t="n">
+        <v>25</v>
       </c>
       <c r="J5">
         <f>Index!$C$2</f>
@@ -607,7 +613,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -620,13 +626,13 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" t="n">
-        <v>2035.93</v>
+        <v>2016.28</v>
       </c>
       <c r="F6" t="n">
-        <v>4071.86</v>
+        <v>6048.84</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -640,7 +646,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>46050</v>
+        <v>46057</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -653,13 +659,13 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7" t="n">
-        <v>1972.59</v>
+        <v>2035.93</v>
       </c>
       <c r="F7" t="n">
-        <v>5917.77</v>
+        <v>4071.86</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -673,7 +679,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>46049</v>
+        <v>46050</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -689,10 +695,10 @@
         <v>3</v>
       </c>
       <c r="E8" t="n">
-        <v>1998.27</v>
+        <v>1972.59</v>
       </c>
       <c r="F8" t="n">
-        <v>5994.81</v>
+        <v>5917.77</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -706,7 +712,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>46044</v>
+        <v>46049</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -722,10 +728,10 @@
         <v>3</v>
       </c>
       <c r="E9" t="n">
-        <v>2010.26</v>
+        <v>1998.27</v>
       </c>
       <c r="F9" t="n">
-        <v>6030.78</v>
+        <v>5994.81</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -739,7 +745,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>46038</v>
+        <v>46044</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -755,10 +761,10 @@
         <v>3</v>
       </c>
       <c r="E10" t="n">
-        <v>2008.74</v>
+        <v>2010.26</v>
       </c>
       <c r="F10" t="n">
-        <v>6026.22</v>
+        <v>6030.78</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -772,7 +778,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>46034</v>
+        <v>46038</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -785,13 +791,13 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E11" t="n">
-        <v>2019.62</v>
+        <v>2008.74</v>
       </c>
       <c r="F11" t="n">
-        <v>10098.1</v>
+        <v>6026.22</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -805,7 +811,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>46030</v>
+        <v>46034</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -818,13 +824,13 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E12" t="n">
-        <v>2082.44</v>
+        <v>2019.62</v>
       </c>
       <c r="F12" t="n">
-        <v>6247.32</v>
+        <v>10098.1</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -838,7 +844,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>46027</v>
+        <v>46030</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -854,10 +860,10 @@
         <v>3</v>
       </c>
       <c r="E13" t="n">
-        <v>2117</v>
+        <v>2082.44</v>
       </c>
       <c r="F13" t="n">
-        <v>6351</v>
+        <v>6247.32</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -871,7 +877,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>46022</v>
+        <v>46027</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -884,13 +890,13 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14" t="n">
-        <v>2110.84</v>
+        <v>2117</v>
       </c>
       <c r="F14" t="n">
-        <v>4221.68</v>
+        <v>6351</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -904,7 +910,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>46020</v>
+        <v>46022</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -920,10 +926,10 @@
         <v>2</v>
       </c>
       <c r="E15" t="n">
-        <v>2111.74</v>
+        <v>2110.84</v>
       </c>
       <c r="F15" t="n">
-        <v>4223.48</v>
+        <v>4221.68</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -937,7 +943,7 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>46017</v>
+        <v>46020</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -953,10 +959,10 @@
         <v>2</v>
       </c>
       <c r="E16" t="n">
-        <v>2131.09</v>
+        <v>2111.74</v>
       </c>
       <c r="F16" t="n">
-        <v>4262.18</v>
+        <v>4223.48</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -970,7 +976,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>46014</v>
+        <v>46017</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -986,10 +992,10 @@
         <v>2</v>
       </c>
       <c r="E17" t="n">
-        <v>2147.11</v>
+        <v>2131.09</v>
       </c>
       <c r="F17" t="n">
-        <v>4294.22</v>
+        <v>4262.18</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1003,7 +1009,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>46009</v>
+        <v>46014</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1019,17 +1025,50 @@
         <v>2</v>
       </c>
       <c r="E18" t="n">
+        <v>2147.11</v>
+      </c>
+      <c r="F18" t="n">
+        <v>4294.22</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>~</t>
+        </is>
+      </c>
+      <c r="J18">
+        <f>Index!$C$2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>46009</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" t="n">
         <v>2120.93</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F19" t="n">
         <v>4241.86</v>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
-      <c r="J18">
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>~</t>
+        </is>
+      </c>
+      <c r="J19">
         <f>Index!$C$2</f>
         <v/>
       </c>

</xml_diff>